<commit_message>
working on range of years
</commit_message>
<xml_diff>
--- a/data/Microfinance/CODEBOOK_mix-market-financial-performance-field-definitions.xlsx
+++ b/data/Microfinance/CODEBOOK_mix-market-financial-performance-field-definitions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NandhiniSridhar/Desktop/honors_thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NandhiniSridhar/Desktop/econ_honors_thesis/data/Microfinance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F8F26D-9DF4-BC48-BEAE-4F3EEB9D22D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE729DEA-7FA8-CE4E-9630-40E76FAF461D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1460" yWindow="1740" windowWidth="26940" windowHeight="15500" tabRatio="266" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2058,10 +2058,10 @@
   <dimension ref="A1:E271"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B264" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A139" sqref="A139:XFD139"/>
+      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6711,6 +6711,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_ExpireDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002F6EF0B8F19DFE4C82A25CD4ECE73C8E" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c8eb6e1bc5699f8cb7427e092b7fa68c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6c756502-b331-4cf9-99aa-897e584036a8" xmlns:ns3="32dc3e3b-d76c-4d37-83cc-97e4babfd09e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f604c76b9bc13ab0d97140661084337" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6952,24 +6969,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C07F869-ABEA-4418-838D-F54E2C481972}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="6c756502-b331-4cf9-99aa-897e584036a8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="32dc3e3b-d76c-4d37-83cc-97e4babfd09e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_ExpireDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19792919-C00A-4092-A410-36239ABD2DE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99B8F0A9-D157-4855-B547-C0C8E82282EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6987,30 +7013,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19792919-C00A-4092-A410-36239ABD2DE2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C07F869-ABEA-4418-838D-F54E2C481972}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="6c756502-b331-4cf9-99aa-897e584036a8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="32dc3e3b-d76c-4d37-83cc-97e4babfd09e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>